<commit_message>
Updated draft spreadsheet and week 2 stats 2020
</commit_message>
<xml_diff>
--- a/2020 Draft Results.xlsx
+++ b/2020 Draft Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcappleman/projects/dke-fantasy-football/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE4E89FF-E7DF-9541-A302-C0D9123E6DEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C87C83CE-A195-9B4C-8FEC-73F2F5FF680C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="20700" windowHeight="19340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20700" windowHeight="19340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All Picks" sheetId="1" r:id="rId1"/>
@@ -1003,15 +1003,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G181"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.1640625" customWidth="1"/>
     <col min="5" max="5" width="32.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5" customWidth="1"/>
+    <col min="6" max="6" width="11.5" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7563,7 +7563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>

</xml_diff>